<commit_message>
working on teeth pattern
</commit_message>
<xml_diff>
--- a/terms/calcaneusTerms.xlsx
+++ b/terms/calcaneusTerms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F9EFC2-F255-BE43-930B-01854CBFA1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF22C5E4-698C-7D4B-A105-578D7580B670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16640" activeTab="1" xr2:uid="{DB14F8C6-EED1-CF49-9D06-87D4724512D6}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16640" activeTab="2" xr2:uid="{DB14F8C6-EED1-CF49-9D06-87D4724512D6}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44122A0-5647-0748-B10B-132650BF5C67}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -940,13 +940,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DB0C01-8443-2A48-8408-BBDE1BFB448B}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -971,6 +976,51 @@
       </c>
       <c r="C2" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding more info to talus
</commit_message>
<xml_diff>
--- a/terms/calcaneusTerms.xlsx
+++ b/terms/calcaneusTerms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3460CB9-D1E8-1349-9B3E-17FCE5EE475E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9868971D-B240-5C4F-93D7-0534D2E143D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{DB14F8C6-EED1-CF49-9D06-87D4724512D6}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16640" xr2:uid="{DB14F8C6-EED1-CF49-9D06-87D4724512D6}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -655,7 +655,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,6 +785,9 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>56</v>
       </c>
@@ -839,6 +842,9 @@
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
adding synonyms to calcaneus terms
</commit_message>
<xml_diff>
--- a/terms/calcaneusTerms.xlsx
+++ b/terms/calcaneusTerms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9868971D-B240-5C4F-93D7-0534D2E143D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97409D2-9758-5543-882F-A455559EDFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16640" xr2:uid="{DB14F8C6-EED1-CF49-9D06-87D4724512D6}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -66,9 +66,6 @@
     <t>GB</t>
   </si>
   <si>
-    <t>calcaneus width ML</t>
-  </si>
-  <si>
     <t>calcaneus distal breadth</t>
   </si>
   <si>
@@ -93,18 +90,12 @@
     <t>Eisenmann</t>
   </si>
   <si>
-    <t>calcaneus maximal depth</t>
-  </si>
-  <si>
     <t>calcanus distal depth</t>
   </si>
   <si>
     <t>CALD</t>
   </si>
   <si>
-    <t>calcaneus lateral depth</t>
-  </si>
-  <si>
     <t>Purdue 1987</t>
   </si>
   <si>
@@ -201,6 +192,9 @@
     <t>calcaneus proximal breadth</t>
   </si>
   <si>
+    <t>calcaneus proximal depth</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
@@ -277,6 +271,24 @@
   </si>
   <si>
     <t>calcaneus minimal breadth; Calcaneum LB [change to Bc]; Calcaneus Bc, mm</t>
+  </si>
+  <si>
+    <t>calcaneus distal width ML (non-plantigrade); calcaneus anteiror width ML (plantigrade); calcaneus anterior breadth (plantigrade)</t>
+  </si>
+  <si>
+    <t>calcaneus posterior length (plantigrade)</t>
+  </si>
+  <si>
+    <t>calcaneus posterior breadth (plantigrade); calcaneus posterior width ML (plantigrade); calcaneus proximal width ML</t>
+  </si>
+  <si>
+    <t>calcaneus proximal width AP (non-plantigrade); calcaneus posterior depth (plantigrade); calcaneus posterior width PD (plantigrade)</t>
+  </si>
+  <si>
+    <t>calcaneus lateral depth; calcaneus distal width AP (non-plantigrade); calcaneus anterior depth (plantigrade); calcneus anterior width PD (plantigrade)</t>
+  </si>
+  <si>
+    <t>width AP of calcaneal body (non-plantigrade); width PD of calcaneal body (plantigrade)</t>
   </si>
 </sst>
 </file>
@@ -655,12 +667,14 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
@@ -689,7 +703,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -697,16 +711,16 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -715,10 +729,10 @@
         <v>6</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
@@ -726,25 +740,25 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -752,58 +766,67 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G4" s="1">
         <v>2</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G5" s="1">
         <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="G6" s="1">
         <v>4</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
@@ -812,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -820,13 +843,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
@@ -835,24 +858,27 @@
         <v>7</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -876,71 +902,71 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
         <v>79</v>
       </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -963,7 +989,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,60 +1001,60 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1051,96 +1077,96 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="L1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>